<commit_message>
fixed outlier where ALCR was in ft not m
</commit_message>
<xml_diff>
--- a/data/distances/Steese_spp_dist_2021_raw.xlsx
+++ b/data/distances/Steese_spp_dist_2021_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinehayes/Google Drive/Projects/Reburns/Chapters/Flammabllity/data/distances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA793A8C-26C4-604F-B521-9BCAA5756FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7588C7-6A1D-0B49-85FB-7134E714BDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35280" yWindow="1940" windowWidth="25220" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A923" workbookViewId="0">
-      <selection activeCell="K946" sqref="K946"/>
+    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
+      <selection activeCell="G471" sqref="G471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11578,7 +11578,7 @@
       <c r="E461" t="s">
         <v>18</v>
       </c>
-      <c r="F461">
+      <c r="G461">
         <v>32.5</v>
       </c>
       <c r="H461" t="s">

</xml_diff>